<commit_message>
added data point for BoSL battery monitering
</commit_message>
<xml_diff>
--- a/Board-Hardware/Documentation/BoSL Battery Log Test.xlsx
+++ b/Board-Hardware/Documentation/BoSL Battery Log Test.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\data\My Documents\Monash\Monash-BoSL\Board-Hardware\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\data\My Documents\Monash\Monash-BoSL\Board-Hardware\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCBD0148-3AC3-4A51-A49A-BA8FB1DC8DCF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3AD5F3D-5EF4-41B1-9F28-ED445DD92207}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -84,6 +84,910 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$15</c:f>
+              <c:numCache>
+                <c:formatCode>d\-mmm</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>43734</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43741</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43748</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>4.05</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.01</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.93</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-E6C2-4FE6-AC31-110BC668962E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="363924976"/>
+        <c:axId val="351734384"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="363924976"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="351734384"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="351734384"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="3.6"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="363924976"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>90487</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CB26FA4C-E624-463F-BB23-6F8F9B261FA7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -349,10 +1253,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="Q9" sqref="Q9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -381,7 +1285,16 @@
         <v>4.01</v>
       </c>
     </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>43748</v>
+      </c>
+      <c r="B4">
+        <v>3.93</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added datapoint for BoSL02 test
</commit_message>
<xml_diff>
--- a/Board-Hardware/Documentation/BoSL Battery Log Test.xlsx
+++ b/Board-Hardware/Documentation/BoSL Battery Log Test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\data\My Documents\Monash\Monash-BoSL\Board-Hardware\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3AD5F3D-5EF4-41B1-9F28-ED445DD92207}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3434FD54-761B-4047-945B-D91C8CD86C23}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>Battery</t>
+    <t>Battery (V)</t>
   </si>
 </sst>
 </file>
@@ -100,7 +100,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
@@ -131,12 +131,27 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:prstDash val="dash"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:forward val="60"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$15</c:f>
+              <c:f>Sheet1!$A$2:$A$5</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>43734</c:v>
                 </c:pt>
@@ -146,15 +161,18 @@
                 <c:pt idx="2">
                   <c:v>43748</c:v>
                 </c:pt>
+                <c:pt idx="3">
+                  <c:v>43755</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$15</c:f>
+              <c:f>Sheet1!$B$2:$B$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>4.05</c:v>
                 </c:pt>
@@ -164,13 +182,16 @@
                 <c:pt idx="2">
                   <c:v>3.93</c:v>
                 </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.9</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-E6C2-4FE6-AC31-110BC668962E}"/>
+              <c16:uniqueId val="{00000000-FC3C-4E93-9861-49F9A9BCB228}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -182,13 +203,14 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="363924976"/>
-        <c:axId val="351734384"/>
+        <c:axId val="357495264"/>
+        <c:axId val="200334864"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="363924976"/>
+        <c:axId val="357495264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="43800"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -243,12 +265,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="351734384"/>
+        <c:crossAx val="200334864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="351734384"/>
+        <c:axId val="200334864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="3.6"/>
@@ -306,7 +328,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="363924976"/>
+        <c:crossAx val="357495264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -318,37 +340,6 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -953,23 +944,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>333375</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>14287</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>166687</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>90487</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>52387</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CB26FA4C-E624-463F-BB23-6F8F9B261FA7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A28970EC-1F3E-4EB9-8669-97565FEB9BFA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1253,10 +1244,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q9" sqref="Q9"/>
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1293,6 +1284,14 @@
         <v>3.93</v>
       </c>
     </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>43755</v>
+      </c>
+      <c r="B5">
+        <v>3.9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>